<commit_message>
update to fim levels script
</commit_message>
<xml_diff>
--- a/fim_levels.xlsx
+++ b/fim_levels.xlsx
@@ -633,34 +633,34 @@
         <v>25</v>
       </c>
       <c r="B4" t="n">
-        <v>25.0952944327695</v>
+        <v>24.9224072985305</v>
       </c>
       <c r="C4" t="n">
         <v>21727.7</v>
       </c>
       <c r="D4" t="n">
-        <v>21702.6047055672</v>
+        <v>21702.7775927015</v>
       </c>
       <c r="E4" t="n">
-        <v>0.115632638447005</v>
+        <v>0.114835104364297</v>
       </c>
       <c r="F4" t="n">
-        <v>9.51988190953861</v>
+        <v>9.48127279342025</v>
       </c>
       <c r="G4" t="n">
-        <v>13.5100250743391</v>
+        <v>13.3704799502666</v>
       </c>
       <c r="H4" t="n">
-        <v>-6.13666436551063</v>
+        <v>-6.08808885193253</v>
       </c>
       <c r="I4" t="n">
-        <v>8.20205181440247</v>
+        <v>8.15874340677624</v>
       </c>
       <c r="J4" t="n">
-        <v>4.81448227763735</v>
+        <v>4.79354389970172</v>
       </c>
       <c r="K4" t="n">
-        <v>0.876191422118637</v>
+        <v>0.874129511356216</v>
       </c>
       <c r="L4" t="n">
         <v>0</v>
@@ -672,10 +672,10 @@
         <v>0</v>
       </c>
       <c r="O4" t="n">
-        <v>4.02542640079274</v>
+        <v>4.02505346810979</v>
       </c>
       <c r="P4" t="n">
-        <v>0.553730891810698</v>
+        <v>0.55327525737075</v>
       </c>
       <c r="Q4" t="n">
         <v>0</v>
@@ -690,13 +690,13 @@
         <v>0</v>
       </c>
       <c r="U4" t="n">
-        <v>0.000569378525089148</v>
+        <v>0.000565315715046144</v>
       </c>
       <c r="V4" t="n">
-        <v>1.57647743727603</v>
+        <v>1.55978096928175</v>
       </c>
       <c r="W4" t="n">
-        <v>-3.64482599375808</v>
+        <v>-3.64760501475902</v>
       </c>
     </row>
     <row r="5">
@@ -704,34 +704,34 @@
         <v>26</v>
       </c>
       <c r="B5" t="n">
-        <v>789.355381246358</v>
+        <v>789.186391011501</v>
       </c>
       <c r="C5" t="n">
         <v>19935.4</v>
       </c>
       <c r="D5" t="n">
-        <v>19146.0446187536</v>
+        <v>19146.2136089885</v>
       </c>
       <c r="E5" t="n">
-        <v>4.12281177112259</v>
+        <v>4.12189275189643</v>
       </c>
       <c r="F5" t="n">
-        <v>217.736474231235</v>
+        <v>217.695206111736</v>
       </c>
       <c r="G5" t="n">
-        <v>-128.918174441175</v>
+        <v>-129.044369179027</v>
       </c>
       <c r="H5" t="n">
-        <v>11.1271161376382</v>
+        <v>11.1130300061982</v>
       </c>
       <c r="I5" t="n">
-        <v>689.409965318659</v>
+        <v>689.422524072594</v>
       </c>
       <c r="J5" t="n">
-        <v>35.7545353419157</v>
+        <v>35.7606071406888</v>
       </c>
       <c r="K5" t="n">
-        <v>2.72571701981283</v>
+        <v>2.72631494135558</v>
       </c>
       <c r="L5" t="n">
         <v>264.1345</v>
@@ -743,10 +743,10 @@
         <v>245.574</v>
       </c>
       <c r="O5" t="n">
-        <v>49.6948278194207</v>
+        <v>49.6949359640064</v>
       </c>
       <c r="P5" t="n">
-        <v>48.4498990760476</v>
+        <v>48.4500312028362</v>
       </c>
       <c r="Q5" t="n">
         <v>0</v>
@@ -761,13 +761,13 @@
         <v>9</v>
       </c>
       <c r="U5" t="n">
-        <v>0.00121229042908649</v>
+        <v>0.0012134685798062</v>
       </c>
       <c r="V5" t="n">
-        <v>26.2847017515505</v>
+        <v>26.2895434634631</v>
       </c>
       <c r="W5" t="n">
-        <v>-14.7354279805174</v>
+        <v>-14.7346221083359</v>
       </c>
     </row>
     <row r="6">
@@ -775,34 +775,34 @@
         <v>27</v>
       </c>
       <c r="B6" t="n">
-        <v>934.886123556179</v>
+        <v>934.546968081922</v>
       </c>
       <c r="C6" t="n">
         <v>21684.6</v>
       </c>
       <c r="D6" t="n">
-        <v>20749.7138764438</v>
+        <v>20750.0530319181</v>
       </c>
       <c r="E6" t="n">
-        <v>4.50553742149433</v>
+        <v>4.50382929934872</v>
       </c>
       <c r="F6" t="n">
-        <v>134.982508517024</v>
+        <v>134.886205927482</v>
       </c>
       <c r="G6" t="n">
-        <v>-127.062262672036</v>
+        <v>-127.317003175792</v>
       </c>
       <c r="H6" t="n">
-        <v>34.0419274924056</v>
+        <v>34.1515602215408</v>
       </c>
       <c r="I6" t="n">
-        <v>892.923950218786</v>
+        <v>892.826205108691</v>
       </c>
       <c r="J6" t="n">
-        <v>83.6091475158178</v>
+        <v>83.5618905472822</v>
       </c>
       <c r="K6" t="n">
-        <v>3.16418319935232</v>
+        <v>3.15952956035878</v>
       </c>
       <c r="L6" t="n">
         <v>117.0225</v>
@@ -814,10 +814,10 @@
         <v>462.483</v>
       </c>
       <c r="O6" t="n">
-        <v>72.9278887501451</v>
+        <v>72.9270470580084</v>
       </c>
       <c r="P6" t="n">
-        <v>95.9013080651871</v>
+        <v>95.9002797189389</v>
       </c>
       <c r="Q6" t="n">
         <v>0</v>
@@ -832,13 +832,13 @@
         <v>16.65</v>
       </c>
       <c r="U6" t="n">
-        <v>-0.00132417163812887</v>
+        <v>-0.0013333412159709</v>
       </c>
       <c r="V6" t="n">
-        <v>33.4009147407071</v>
+        <v>33.3632315703542</v>
       </c>
       <c r="W6" t="n">
-        <v>-16.4996678807855</v>
+        <v>-16.5059400050353</v>
       </c>
     </row>
     <row r="7">
@@ -846,34 +846,34 @@
         <v>28</v>
       </c>
       <c r="B7" t="n">
-        <v>758.170846404077</v>
+        <v>757.632598676104</v>
       </c>
       <c r="C7" t="n">
         <v>22068.8</v>
       </c>
       <c r="D7" t="n">
-        <v>21310.6291535959</v>
+        <v>21311.1674013239</v>
       </c>
       <c r="E7" t="n">
-        <v>3.55771216766794</v>
+        <v>3.55509665148159</v>
       </c>
       <c r="F7" t="n">
-        <v>118.085625967881</v>
+        <v>117.918700583147</v>
       </c>
       <c r="G7" t="n">
-        <v>-144.882762736409</v>
+        <v>-145.274238132111</v>
       </c>
       <c r="H7" t="n">
-        <v>4.94757391929594</v>
+        <v>5.13343402588055</v>
       </c>
       <c r="I7" t="n">
-        <v>780.020409253309</v>
+        <v>779.854702199187</v>
       </c>
       <c r="J7" t="n">
-        <v>107.67692517046</v>
+        <v>107.596810543394</v>
       </c>
       <c r="K7" t="n">
-        <v>4.13791966877852</v>
+        <v>4.13003036559169</v>
       </c>
       <c r="L7" t="n">
         <v>63.2366</v>
@@ -885,10 +885,10 @@
         <v>366.6105</v>
       </c>
       <c r="O7" t="n">
-        <v>53.6944150940942</v>
+        <v>53.6929881754041</v>
       </c>
       <c r="P7" t="n">
-        <v>108.305639479666</v>
+        <v>108.303896126702</v>
       </c>
       <c r="Q7" t="n">
         <v>0</v>
@@ -903,13 +903,13 @@
         <v>23.85</v>
       </c>
       <c r="U7" t="n">
-        <v>-0.003027602804626</v>
+        <v>-0.00304314796826921</v>
       </c>
       <c r="V7" t="n">
-        <v>52.0641650048644</v>
+        <v>52.0002808152299</v>
       </c>
       <c r="W7" t="n">
-        <v>-26.3127275617496</v>
+        <v>-26.323360679166</v>
       </c>
     </row>
     <row r="8">
@@ -917,34 +917,34 @@
         <v>29</v>
       </c>
       <c r="B8" t="n">
-        <v>1202.20796564391</v>
+        <v>1201.36961626069</v>
       </c>
       <c r="C8" t="n">
         <v>22656.8</v>
       </c>
       <c r="D8" t="n">
-        <v>21454.5920343561</v>
+        <v>21455.4303837393</v>
       </c>
       <c r="E8" t="n">
-        <v>5.60349953855455</v>
+        <v>5.59937318792347</v>
       </c>
       <c r="F8" t="n">
-        <v>189.759685304435</v>
+        <v>189.510378325602</v>
       </c>
       <c r="G8" t="n">
-        <v>-183.374231604341</v>
+        <v>-184.001523285647</v>
       </c>
       <c r="H8" t="n">
-        <v>-6.5086586025155</v>
+        <v>-6.15590734074753</v>
       </c>
       <c r="I8" t="n">
-        <v>1202.33117054633</v>
+        <v>1202.01666856148</v>
       </c>
       <c r="J8" t="n">
-        <v>170.275815441869</v>
+        <v>170.123762716285</v>
       </c>
       <c r="K8" t="n">
-        <v>4.32499342309285</v>
+        <v>4.31002000192808</v>
       </c>
       <c r="L8" t="n">
         <v>205.2442</v>
@@ -956,10 +956,10 @@
         <v>368.9235</v>
       </c>
       <c r="O8" t="n">
-        <v>51.8924511473711</v>
+        <v>51.8897429418417</v>
       </c>
       <c r="P8" t="n">
-        <v>122.648820751599</v>
+        <v>122.645511972921</v>
       </c>
       <c r="Q8" t="n">
         <v>0</v>
@@ -974,13 +974,13 @@
         <v>30.6</v>
       </c>
       <c r="U8" t="n">
-        <v>0.0876359150838347</v>
+        <v>0.0876064113017144</v>
       </c>
       <c r="V8" t="n">
-        <v>63.5947723692911</v>
+        <v>63.4735240341065</v>
       </c>
       <c r="W8" t="n">
-        <v>-24.3260185019776</v>
+        <v>-24.3461995169037</v>
       </c>
     </row>
     <row r="9">
@@ -988,34 +988,34 @@
         <v>30</v>
       </c>
       <c r="B9" t="n">
-        <v>1099.83650320098</v>
+        <v>1098.70135446708</v>
       </c>
       <c r="C9" t="n">
         <v>23368.9</v>
       </c>
       <c r="D9" t="n">
-        <v>22269.063496799</v>
+        <v>22270.1986455329</v>
       </c>
       <c r="E9" t="n">
-        <v>4.93885386495516</v>
+        <v>4.93350495859841</v>
       </c>
       <c r="F9" t="n">
-        <v>181.15192902779</v>
+        <v>180.798814489675</v>
       </c>
       <c r="G9" t="n">
-        <v>-238.913678931486</v>
+        <v>-239.759508197758</v>
       </c>
       <c r="H9" t="n">
-        <v>-20.2209616501191</v>
+        <v>-19.6326161067901</v>
       </c>
       <c r="I9" t="n">
-        <v>1177.81921475479</v>
+        <v>1177.29466428196</v>
       </c>
       <c r="J9" t="n">
-        <v>164.08123004054</v>
+        <v>163.827624871277</v>
       </c>
       <c r="K9" t="n">
-        <v>4.10499809197086</v>
+        <v>4.08002427453772</v>
       </c>
       <c r="L9" t="n">
         <v>194.0897</v>
@@ -1027,10 +1027,10 @@
         <v>379.138</v>
       </c>
       <c r="O9" t="n">
-        <v>44.0506664336486</v>
+        <v>44.0461494812622</v>
       </c>
       <c r="P9" t="n">
-        <v>148.848204420334</v>
+        <v>148.8426857861</v>
       </c>
       <c r="Q9" t="n">
         <v>2.3513184</v>
@@ -1045,13 +1045,13 @@
         <v>34.65</v>
       </c>
       <c r="U9" t="n">
-        <v>0.46527899758539</v>
+        <v>0.465229788920239</v>
       </c>
       <c r="V9" t="n">
-        <v>57.6872806827532</v>
+        <v>57.4850534326381</v>
       </c>
       <c r="W9" t="n">
-        <v>-11.658830312038</v>
+        <v>-11.6924897527786</v>
       </c>
     </row>
     <row r="10">
@@ -1059,34 +1059,34 @@
         <v>31</v>
       </c>
       <c r="B10" t="n">
-        <v>956.334909920479</v>
+        <v>954.916859954923</v>
       </c>
       <c r="C10" t="n">
         <v>23922</v>
       </c>
       <c r="D10" t="n">
-        <v>22965.6650900795</v>
+        <v>22967.0831400451</v>
       </c>
       <c r="E10" t="n">
-        <v>4.16419427074892</v>
+        <v>4.15776289105665</v>
       </c>
       <c r="F10" t="n">
-        <v>151.12441695879</v>
+        <v>150.657529494469</v>
       </c>
       <c r="G10" t="n">
-        <v>-245.816017313335</v>
+        <v>-246.855442776727</v>
       </c>
       <c r="H10" t="n">
-        <v>-40.4014586271334</v>
+        <v>-39.5874596766627</v>
       </c>
       <c r="I10" t="n">
-        <v>1091.42796890216</v>
+        <v>1090.70223291384</v>
       </c>
       <c r="J10" t="n">
-        <v>163.246974281998</v>
+        <v>162.896101663084</v>
       </c>
       <c r="K10" t="n">
-        <v>4.86720648878867</v>
+        <v>4.83265424069177</v>
       </c>
       <c r="L10" t="n">
         <v>134.3118</v>
@@ -1098,10 +1098,10 @@
         <v>328.578</v>
       </c>
       <c r="O10" t="n">
-        <v>27.022027780874</v>
+        <v>27.0157784015024</v>
       </c>
       <c r="P10" t="n">
-        <v>166.360141117631</v>
+        <v>166.352505872451</v>
       </c>
       <c r="Q10" t="n">
         <v>13.06288</v>
@@ -1116,13 +1116,13 @@
         <v>36.9</v>
       </c>
       <c r="U10" t="n">
-        <v>0.406761392072731</v>
+        <v>0.40669330996989</v>
       </c>
       <c r="V10" t="n">
-        <v>63.6506708428528</v>
+        <v>63.3708815740861</v>
       </c>
       <c r="W10" t="n">
-        <v>-15.7609978020598</v>
+        <v>-15.8075669479418</v>
       </c>
     </row>
     <row r="11">
@@ -1130,34 +1130,34 @@
         <v>32</v>
       </c>
       <c r="B11" t="n">
-        <v>809.809270551149</v>
+        <v>808.032521835996</v>
       </c>
       <c r="C11" t="n">
         <v>24777</v>
       </c>
       <c r="D11" t="n">
-        <v>23967.1907294489</v>
+        <v>23968.967478164</v>
       </c>
       <c r="E11" t="n">
-        <v>3.37882432569006</v>
+        <v>3.37116115899496</v>
       </c>
       <c r="F11" t="n">
-        <v>176.751068114887</v>
+        <v>176.150003453731</v>
       </c>
       <c r="G11" t="n">
-        <v>-297.578884743394</v>
+        <v>-298.874385133037</v>
       </c>
       <c r="H11" t="n">
-        <v>-55.6446409070309</v>
+        <v>-54.5396431924389</v>
       </c>
       <c r="I11" t="n">
-        <v>986.281728086686</v>
+        <v>985.296546707741</v>
       </c>
       <c r="J11" t="n">
-        <v>179.408589461989</v>
+        <v>178.932282408045</v>
       </c>
       <c r="K11" t="n">
-        <v>5.24621056803551</v>
+        <v>5.19930614001504</v>
       </c>
       <c r="L11" t="n">
         <v>114.6509</v>
@@ -1169,10 +1169,10 @@
         <v>272.843</v>
       </c>
       <c r="O11" t="n">
-        <v>19.0938018374399</v>
+        <v>19.0853183499375</v>
       </c>
       <c r="P11" t="n">
-        <v>173.759285639595</v>
+        <v>173.748920849235</v>
       </c>
       <c r="Q11" t="n">
         <v>16.12079192</v>
@@ -1187,13 +1187,13 @@
         <v>39.15</v>
       </c>
       <c r="U11" t="n">
-        <v>0.382636379935672</v>
+        <v>0.382543958971247</v>
       </c>
       <c r="V11" t="n">
-        <v>65.7777556275321</v>
+        <v>65.3979437096223</v>
       </c>
       <c r="W11" t="n">
-        <v>-17.706444947841</v>
+        <v>-17.7696622280848</v>
       </c>
     </row>
     <row r="12">
@@ -1201,34 +1201,34 @@
         <v>33</v>
       </c>
       <c r="B12" t="n">
-        <v>596.847177846712</v>
+        <v>594.598717895733</v>
       </c>
       <c r="C12" t="n">
         <v>25215.5</v>
       </c>
       <c r="D12" t="n">
-        <v>24618.6528221533</v>
+        <v>24620.9012821043</v>
       </c>
       <c r="E12" t="n">
-        <v>2.42436977424547</v>
+        <v>2.41501605113017</v>
       </c>
       <c r="F12" t="n">
-        <v>157.115398497924</v>
+        <v>156.33169683825</v>
       </c>
       <c r="G12" t="n">
-        <v>-340.612706022441</v>
+        <v>-342.236420578448</v>
       </c>
       <c r="H12" t="n">
-        <v>-109.363942956686</v>
+        <v>-107.897980003754</v>
       </c>
       <c r="I12" t="n">
-        <v>889.708428327915</v>
+        <v>888.401421639685</v>
       </c>
       <c r="J12" t="n">
-        <v>139.323276175985</v>
+        <v>138.69137577829</v>
       </c>
       <c r="K12" t="n">
-        <v>5.49737875854308</v>
+        <v>5.43515224630829</v>
       </c>
       <c r="L12" t="n">
         <v>112.7448</v>
@@ -1240,10 +1240,10 @@
         <v>218.928</v>
       </c>
       <c r="O12" t="n">
-        <v>10.7214812657096</v>
+        <v>10.7102265108572</v>
       </c>
       <c r="P12" t="n">
-        <v>169.656673704416</v>
+        <v>169.642923088934</v>
       </c>
       <c r="Q12" t="n">
         <v>14.371564</v>
@@ -1258,13 +1258,13 @@
         <v>40.95</v>
       </c>
       <c r="U12" t="n">
-        <v>0.353138799436806</v>
+        <v>0.353016187681024</v>
       </c>
       <c r="V12" t="n">
-        <v>71.4901455336305</v>
+        <v>70.9862619568728</v>
       </c>
       <c r="W12" t="n">
-        <v>-23.279941509806</v>
+        <v>-23.363809729259</v>
       </c>
     </row>
     <row r="13">
@@ -1272,34 +1272,34 @@
         <v>34</v>
       </c>
       <c r="B13" t="n">
-        <v>322.183454128687</v>
+        <v>319.226980099585</v>
       </c>
       <c r="C13" t="n">
         <v>25805.8</v>
       </c>
       <c r="D13" t="n">
-        <v>25483.6165458713</v>
+        <v>25486.5730199004</v>
       </c>
       <c r="E13" t="n">
-        <v>1.2642768091756</v>
+        <v>1.25253002767507</v>
       </c>
       <c r="F13" t="n">
-        <v>191.420115438359</v>
+        <v>190.402666050689</v>
       </c>
       <c r="G13" t="n">
-        <v>-421.202812492363</v>
+        <v>-423.341655978137</v>
       </c>
       <c r="H13" t="n">
-        <v>-184.648876972184</v>
+        <v>-182.806061757228</v>
       </c>
       <c r="I13" t="n">
-        <v>736.615028154875</v>
+        <v>734.972031784261</v>
       </c>
       <c r="J13" t="n">
-        <v>144.926154090373</v>
+        <v>144.131812279155</v>
       </c>
       <c r="K13" t="n">
-        <v>7.1044795956613</v>
+        <v>7.02625663423476</v>
       </c>
       <c r="L13" t="n">
         <v>52.3712</v>
@@ -1311,10 +1311,10 @@
         <v>134.724</v>
       </c>
       <c r="O13" t="n">
-        <v>-0.424905321282377</v>
+        <v>-0.439053314204816</v>
       </c>
       <c r="P13" t="n">
-        <v>159.568078790543</v>
+        <v>159.550793330925</v>
       </c>
       <c r="Q13" t="n">
         <v>16.24578</v>
@@ -1329,13 +1329,13 @@
         <v>40.95</v>
       </c>
       <c r="U13" t="n">
-        <v>0.313889240225479</v>
+        <v>0.313735108902695</v>
       </c>
       <c r="V13" t="n">
-        <v>69.4967347870356</v>
+        <v>68.8633188334068</v>
       </c>
       <c r="W13" t="n">
-        <v>-26.1741426276803</v>
+        <v>-26.2795706881577</v>
       </c>
     </row>
     <row r="14">
@@ -1343,34 +1343,34 @@
         <v>35</v>
       </c>
       <c r="B14" t="n">
-        <v>182.855273462856</v>
+        <v>179.762134886624</v>
       </c>
       <c r="C14" t="n">
         <v>26272</v>
       </c>
       <c r="D14" t="n">
-        <v>26089.1447265371</v>
+        <v>26092.2378651134</v>
       </c>
       <c r="E14" t="n">
-        <v>0.700886423757918</v>
+        <v>0.688948705036041</v>
       </c>
       <c r="F14" t="n">
-        <v>160.182790537529</v>
+        <v>159.030597474995</v>
       </c>
       <c r="G14" t="n">
-        <v>-397.59718612988</v>
+        <v>-399.765233904761</v>
       </c>
       <c r="H14" t="n">
-        <v>-228.723914592675</v>
+        <v>-226.629479987968</v>
       </c>
       <c r="I14" t="n">
-        <v>648.993583647882</v>
+        <v>647.126251304359</v>
       </c>
       <c r="J14" t="n">
-        <v>120.602873793211</v>
+        <v>119.700071947492</v>
       </c>
       <c r="K14" t="n">
-        <v>13.2628001444019</v>
+        <v>13.1738965603828</v>
       </c>
       <c r="L14" t="n">
         <v>51.4976</v>
@@ -1382,10 +1382,10 @@
         <v>76.057</v>
       </c>
       <c r="O14" t="n">
-        <v>-4.45217764032489</v>
+        <v>-4.4682574109516</v>
       </c>
       <c r="P14" t="n">
-        <v>149.859353341593</v>
+        <v>149.839707712184</v>
       </c>
       <c r="Q14" t="n">
         <v>18.119996</v>
@@ -1400,13 +1400,13 @@
         <v>40.95</v>
       </c>
       <c r="U14" t="n">
-        <v>0.312108308287221</v>
+        <v>0.311933131756504</v>
       </c>
       <c r="V14" t="n">
-        <v>75.9521631615708</v>
+        <v>75.2322601123194</v>
       </c>
       <c r="W14" t="n">
-        <v>-30.3225498608576</v>
+        <v>-30.4423731488243</v>
       </c>
     </row>
     <row r="15">
@@ -1414,34 +1414,34 @@
         <v>36</v>
       </c>
       <c r="B15" t="n">
-        <v>174.908785484829</v>
+        <v>171.674844261704</v>
       </c>
       <c r="C15" t="n">
         <v>26734.3</v>
       </c>
       <c r="D15" t="n">
-        <v>26559.3912145152</v>
+        <v>26562.6251557383</v>
       </c>
       <c r="E15" t="n">
-        <v>0.658557208906352</v>
+        <v>0.646302250832376</v>
       </c>
       <c r="F15" t="n">
-        <v>151.726416215019</v>
+        <v>150.463039238742</v>
       </c>
       <c r="G15" t="n">
-        <v>-354.358633055488</v>
+        <v>-356.580211254019</v>
       </c>
       <c r="H15" t="n">
-        <v>-260.224029610304</v>
+        <v>-257.909071124536</v>
       </c>
       <c r="I15" t="n">
-        <v>637.765031935603</v>
+        <v>635.701087401517</v>
       </c>
       <c r="J15" t="n">
-        <v>119.869580185206</v>
+        <v>118.871721961791</v>
       </c>
       <c r="K15" t="n">
-        <v>31.5602243446566</v>
+        <v>31.4619600657064</v>
       </c>
       <c r="L15" t="n">
         <v>51.2176</v>
@@ -1453,10 +1453,10 @@
         <v>52.018</v>
       </c>
       <c r="O15" t="n">
-        <v>-5.98465604405151</v>
+        <v>-6.00242886034181</v>
       </c>
       <c r="P15" t="n">
-        <v>145.863686810169</v>
+        <v>145.841972684358</v>
       </c>
       <c r="Q15" t="n">
         <v>16.093332</v>
@@ -1471,13 +1471,13 @@
         <v>40.95</v>
       </c>
       <c r="U15" t="n">
-        <v>0.310793582602451</v>
+        <v>0.310599961662757</v>
       </c>
       <c r="V15" t="n">
-        <v>79.2175813112917</v>
+        <v>78.4218793738578</v>
       </c>
       <c r="W15" t="n">
-        <v>-25.1761402542718</v>
+        <v>-25.3085797855169</v>
       </c>
     </row>
     <row r="16">
@@ -1485,34 +1485,34 @@
         <v>37</v>
       </c>
       <c r="B16" t="n">
-        <v>182.569747769379</v>
+        <v>179.334934991508</v>
       </c>
       <c r="C16" t="n">
         <v>27164.4</v>
       </c>
       <c r="D16" t="n">
-        <v>26981.8302522306</v>
+        <v>26985.0650650085</v>
       </c>
       <c r="E16" t="n">
-        <v>0.676639598065387</v>
+        <v>0.66457106758675</v>
       </c>
       <c r="F16" t="n">
-        <v>152.650774234086</v>
+        <v>151.28585061559</v>
       </c>
       <c r="G16" t="n">
-        <v>-321.706826503428</v>
+        <v>-323.851732381854</v>
       </c>
       <c r="H16" t="n">
-        <v>-223.222422936206</v>
+        <v>-220.686100619346</v>
       </c>
       <c r="I16" t="n">
-        <v>574.848222974927</v>
+        <v>572.586917377118</v>
       </c>
       <c r="J16" t="n">
-        <v>114.672760438372</v>
+        <v>113.579483778479</v>
       </c>
       <c r="K16" t="n">
-        <v>34.5568089317633</v>
+        <v>34.4491483040743</v>
       </c>
       <c r="L16" t="n">
         <v>18.424</v>
@@ -1524,10 +1524,10 @@
         <v>27.457</v>
       </c>
       <c r="O16" t="n">
-        <v>-7.56128630652472</v>
+        <v>-7.58075861709429</v>
       </c>
       <c r="P16" t="n">
-        <v>142.938159743719</v>
+        <v>142.914369242842</v>
       </c>
       <c r="Q16" t="n">
         <v>14.066668</v>
@@ -1542,13 +1542,13 @@
         <v>40.95</v>
       </c>
       <c r="U16" t="n">
-        <v>0.296652202535351</v>
+        <v>0.296440066934054</v>
       </c>
       <c r="V16" t="n">
-        <v>83.8403756342591</v>
+        <v>82.9685860994186</v>
       </c>
       <c r="W16" t="n">
-        <v>-18.7175372691963</v>
+        <v>-18.8626410975357</v>
       </c>
     </row>
     <row r="17">
@@ -1556,34 +1556,34 @@
         <v>38</v>
       </c>
       <c r="B17" t="n">
-        <v>150.273537972626</v>
+        <v>147.120625920395</v>
       </c>
       <c r="C17" t="n">
         <v>27453.8</v>
       </c>
       <c r="D17" t="n">
-        <v>27303.5264620274</v>
+        <v>27306.6793740796</v>
       </c>
       <c r="E17" t="n">
-        <v>0.550381424837632</v>
+        <v>0.538771572716557</v>
       </c>
       <c r="F17" t="n">
-        <v>132.993446785802</v>
+        <v>131.553802420048</v>
       </c>
       <c r="G17" t="n">
-        <v>-291.430644759636</v>
+        <v>-293.437465750915</v>
       </c>
       <c r="H17" t="n">
-        <v>-189.148506983371</v>
+        <v>-186.441232310292</v>
       </c>
       <c r="I17" t="n">
-        <v>497.859242929832</v>
+        <v>495.445521561555</v>
       </c>
       <c r="J17" t="n">
-        <v>109.535971374261</v>
+        <v>108.36900604327</v>
       </c>
       <c r="K17" t="n">
-        <v>34.400370688136</v>
+        <v>34.2854535545002</v>
       </c>
       <c r="L17" t="n">
         <v>2.1784</v>
@@ -1595,10 +1595,10 @@
         <v>9.157</v>
       </c>
       <c r="O17" t="n">
-        <v>-6.51828147506779</v>
+        <v>-6.5390662518609</v>
       </c>
       <c r="P17" t="n">
-        <v>121.091188327398</v>
+        <v>121.065794307066</v>
       </c>
       <c r="Q17" t="n">
         <v>14.28301</v>
@@ -1613,13 +1613,13 @@
         <v>40.95</v>
       </c>
       <c r="U17" t="n">
-        <v>0.242083548161559</v>
+        <v>0.241857114266769</v>
       </c>
       <c r="V17" t="n">
-        <v>94.2603131309895</v>
+        <v>93.329763526848</v>
       </c>
       <c r="W17" t="n">
-        <v>-10.3317790640474</v>
+        <v>-10.4866631325346</v>
       </c>
     </row>
     <row r="18">
@@ -1627,34 +1627,34 @@
         <v>39</v>
       </c>
       <c r="B18" t="n">
-        <v>161.399971345885</v>
+        <v>157.979372686385</v>
       </c>
       <c r="C18" t="n">
         <v>27967.7</v>
       </c>
       <c r="D18" t="n">
-        <v>27806.3000286541</v>
+        <v>27809.7206273136</v>
       </c>
       <c r="E18" t="n">
-        <v>0.580443896453553</v>
+        <v>0.568072490923277</v>
       </c>
       <c r="F18" t="n">
-        <v>125.622152498091</v>
+        <v>124.063139403081</v>
       </c>
       <c r="G18" t="n">
-        <v>-244.400592151977</v>
+        <v>-246.573249825288</v>
       </c>
       <c r="H18" t="n">
-        <v>-176.47845404813</v>
+        <v>-173.60961343917</v>
       </c>
       <c r="I18" t="n">
-        <v>456.656865047901</v>
+        <v>454.099096547763</v>
       </c>
       <c r="J18" t="n">
-        <v>108.934183480044</v>
+        <v>107.69757547566</v>
       </c>
       <c r="K18" t="n">
-        <v>29.9060656369812</v>
+        <v>29.7842904277946</v>
       </c>
       <c r="L18" t="n">
         <v>0</v>
@@ -1666,10 +1666,10 @@
         <v>0.67</v>
       </c>
       <c r="O18" t="n">
-        <v>-4.06523009208735</v>
+        <v>-4.08725527198697</v>
       </c>
       <c r="P18" t="n">
-        <v>97.8998066730462</v>
+        <v>97.8728971771319</v>
       </c>
       <c r="Q18" t="n">
         <v>14.499352</v>
@@ -1684,13 +1684,13 @@
         <v>32.3663016</v>
       </c>
       <c r="U18" t="n">
-        <v>0.240982025767556</v>
+        <v>0.240742078650597</v>
       </c>
       <c r="V18" t="n">
-        <v>90.0215042472321</v>
+        <v>89.0354208920562</v>
       </c>
       <c r="W18" t="n">
-        <v>5.09154947691755</v>
+        <v>4.92742216845662</v>
       </c>
     </row>
     <row r="19">
@@ -1698,34 +1698,34 @@
         <v>40</v>
       </c>
       <c r="B19" t="n">
-        <v>135.152029957927</v>
+        <v>131.63166888008</v>
       </c>
       <c r="C19" t="n">
         <v>28297</v>
       </c>
       <c r="D19" t="n">
-        <v>28161.8479700421</v>
+        <v>28165.3683311199</v>
       </c>
       <c r="E19" t="n">
-        <v>0.479911794501908</v>
+        <v>0.467352911322094</v>
       </c>
       <c r="F19" t="n">
-        <v>129.399589367791</v>
+        <v>127.734894894319</v>
       </c>
       <c r="G19" t="n">
-        <v>-230.138091038824</v>
+        <v>-232.316595300956</v>
       </c>
       <c r="H19" t="n">
-        <v>-177.641757108277</v>
+        <v>-174.664409553126</v>
       </c>
       <c r="I19" t="n">
-        <v>413.532288737237</v>
+        <v>410.877778839843</v>
       </c>
       <c r="J19" t="n">
-        <v>96.8532639268296</v>
+        <v>95.5698842203951</v>
       </c>
       <c r="K19" t="n">
-        <v>13.9029145053357</v>
+        <v>13.7765334438653</v>
       </c>
       <c r="L19" t="n">
         <v>0</v>
@@ -1737,10 +1737,10 @@
         <v>0.174</v>
       </c>
       <c r="O19" t="n">
-        <v>-2.45097950153999</v>
+        <v>-2.47383773051272</v>
       </c>
       <c r="P19" t="n">
-        <v>87.9682634017112</v>
+        <v>87.9403361193028</v>
       </c>
       <c r="Q19" t="n">
         <v>14.261254</v>
@@ -1755,13 +1755,13 @@
         <v>25.07397996</v>
       </c>
       <c r="U19" t="n">
-        <v>0.240656163080453</v>
+        <v>0.240407140545074</v>
       </c>
       <c r="V19" t="n">
-        <v>94.9461107733805</v>
+        <v>93.9227312041082</v>
       </c>
       <c r="W19" t="n">
-        <v>9.39966550843977</v>
+        <v>9.22933048213906</v>
       </c>
     </row>
     <row r="20">
@@ -1769,34 +1769,34 @@
         <v>41</v>
       </c>
       <c r="B20" t="n">
-        <v>139.262474981548</v>
+        <v>135.478203984032</v>
       </c>
       <c r="C20" t="n">
         <v>28624.1</v>
       </c>
       <c r="D20" t="n">
-        <v>28484.8375250185</v>
+        <v>28488.621796016</v>
       </c>
       <c r="E20" t="n">
-        <v>0.488900366236011</v>
+        <v>0.47555197634368</v>
       </c>
       <c r="F20" t="n">
-        <v>115.584695944007</v>
+        <v>113.798803098809</v>
       </c>
       <c r="G20" t="n">
-        <v>-221.001690386205</v>
+        <v>-223.345888356218</v>
       </c>
       <c r="H20" t="n">
-        <v>-137.697885312768</v>
+        <v>-134.508586406658</v>
       </c>
       <c r="I20" t="n">
-        <v>382.377354736514</v>
+        <v>379.533875648099</v>
       </c>
       <c r="J20" t="n">
-        <v>95.5583478848941</v>
+        <v>94.183606972711</v>
       </c>
       <c r="K20" t="n">
-        <v>12.312265548904</v>
+        <v>12.176887675265</v>
       </c>
       <c r="L20" t="n">
         <v>0</v>
@@ -1808,10 +1808,10 @@
         <v>0.08</v>
       </c>
       <c r="O20" t="n">
-        <v>-1.56283132523353</v>
+        <v>-1.58731678529755</v>
       </c>
       <c r="P20" t="n">
-        <v>79.5581605698576</v>
+        <v>79.5282452006957</v>
       </c>
       <c r="Q20" t="n">
         <v>14.023156</v>
@@ -1826,13 +1826,13 @@
         <v>18.30645234</v>
       </c>
       <c r="U20" t="n">
-        <v>0.204647570987417</v>
+        <v>0.204380821041376</v>
       </c>
       <c r="V20" t="n">
-        <v>88.6052380279684</v>
+        <v>87.5090061368787</v>
       </c>
       <c r="W20" t="n">
-        <v>15.5706481191361</v>
+        <v>15.3881872868046</v>
       </c>
     </row>
     <row r="21">
@@ -1840,34 +1840,34 @@
         <v>42</v>
       </c>
       <c r="B21" t="n">
-        <v>149.245729718508</v>
+        <v>148.653550797441</v>
       </c>
       <c r="C21" t="n">
         <v>29016.7</v>
       </c>
       <c r="D21" t="n">
-        <v>28867.4542702815</v>
+        <v>28868.0464492026</v>
       </c>
       <c r="E21" t="n">
-        <v>0.517003433420693</v>
+        <v>0.514941497891153</v>
       </c>
       <c r="F21" t="n">
-        <v>127.800809110679</v>
+        <v>125.921166453252</v>
       </c>
       <c r="G21" t="n">
-        <v>-222.349844632279</v>
+        <v>-224.774256360233</v>
       </c>
       <c r="H21" t="n">
-        <v>-107.167739633304</v>
+        <v>-100.463923798247</v>
       </c>
       <c r="I21" t="n">
-        <v>350.962504873412</v>
+        <v>347.970564502669</v>
       </c>
       <c r="J21" t="n">
-        <v>105.532921827368</v>
+        <v>104.086404126137</v>
       </c>
       <c r="K21" t="n">
-        <v>13.2167759181005</v>
+        <v>13.0743298114645</v>
       </c>
       <c r="L21" t="n">
         <v>0</v>
@@ -1879,10 +1879,10 @@
         <v>0.035</v>
       </c>
       <c r="O21" t="n">
-        <v>-0.903063713400726</v>
+        <v>-0.928827587227062</v>
       </c>
       <c r="P21" t="n">
-        <v>57.2464701729108</v>
+        <v>57.2149928882472</v>
       </c>
       <c r="Q21" t="n">
         <v>13.04705068</v>
@@ -1897,13 +1897,13 @@
         <v>11.95799418</v>
       </c>
       <c r="U21" t="n">
-        <v>0.0594993802555712</v>
+        <v>0.0592187029909824</v>
       </c>
       <c r="V21" t="n">
-        <v>87.3190165880906</v>
+        <v>86.1655491812051</v>
       </c>
       <c r="W21" t="n">
-        <v>16.0501798400874</v>
+        <v>15.8581925198514</v>
       </c>
     </row>
     <row r="22">
@@ -1911,34 +1911,34 @@
         <v>43</v>
       </c>
       <c r="B22" t="n">
-        <v>181.703019237481</v>
+        <v>186.39827160409</v>
       </c>
       <c r="C22" t="n">
-        <v>29349.9</v>
+        <v>29374.9</v>
       </c>
       <c r="D22" t="n">
-        <v>29168.1969807625</v>
+        <v>29188.5017283959</v>
       </c>
       <c r="E22" t="n">
-        <v>0.622949095404568</v>
+        <v>0.638601711518305</v>
       </c>
       <c r="F22" t="n">
-        <v>178.237287370114</v>
+        <v>173.201300645855</v>
       </c>
       <c r="G22" t="n">
-        <v>-238.154044327949</v>
+        <v>-236.634103769505</v>
       </c>
       <c r="H22" t="n">
-        <v>-103.681291012186</v>
+        <v>-91.3932639132929</v>
       </c>
       <c r="I22" t="n">
-        <v>345.301067207502</v>
+        <v>341.224338641033</v>
       </c>
       <c r="J22" t="n">
-        <v>120.887158823903</v>
+        <v>119.331776450609</v>
       </c>
       <c r="K22" t="n">
-        <v>15.1322552008175</v>
+        <v>15.8724415494483</v>
       </c>
       <c r="L22" t="n">
         <v>0</v>
@@ -1950,10 +1950,10 @@
         <v>0.012</v>
       </c>
       <c r="O22" t="n">
-        <v>-0.342321680390143</v>
+        <v>-0.371226778934691</v>
       </c>
       <c r="P22" t="n">
-        <v>36.5336870449392</v>
+        <v>36.4983719358353</v>
       </c>
       <c r="Q22" t="n">
         <v>8.517842</v>
@@ -1968,13 +1968,13 @@
         <v>8.18345387</v>
       </c>
       <c r="U22" t="n">
-        <v>0.0573461887951549</v>
+        <v>0.0570312903428941</v>
       </c>
       <c r="V22" t="n">
-        <v>103.021088165181</v>
+        <v>101.726985838462</v>
       </c>
       <c r="W22" t="n">
-        <v>17.8873275942558</v>
+        <v>15.9844324852698</v>
       </c>
     </row>
     <row r="23">
@@ -1982,34 +1982,34 @@
         <v>44</v>
       </c>
       <c r="B23" t="n">
-        <v>162.522101396599</v>
+        <v>173.289336441366</v>
       </c>
       <c r="C23" t="n">
-        <v>29641.2825253979</v>
+        <v>29666.5307226025</v>
       </c>
       <c r="D23" t="n">
-        <v>29478.7604240013</v>
+        <v>29493.2413861611</v>
       </c>
       <c r="E23" t="n">
-        <v>0.55131931960164</v>
+        <v>0.587556091826102</v>
       </c>
       <c r="F23" t="n">
-        <v>150.816686534242</v>
+        <v>145.649351581627</v>
       </c>
       <c r="G23" t="n">
-        <v>-247.670807688072</v>
+        <v>-246.221519331698</v>
       </c>
       <c r="H23" t="n">
-        <v>-100.749973179488</v>
+        <v>-84.3691353918696</v>
       </c>
       <c r="I23" t="n">
-        <v>360.126195729917</v>
+        <v>358.230639583307</v>
       </c>
       <c r="J23" t="n">
-        <v>134.470938035208</v>
+        <v>132.480991083331</v>
       </c>
       <c r="K23" t="n">
-        <v>17.8369291566928</v>
+        <v>18.5276746001496</v>
       </c>
       <c r="L23" t="n">
         <v>0</v>
@@ -2021,10 +2021,10 @@
         <v>0</v>
       </c>
       <c r="O23" t="n">
-        <v>-0.124745015508402</v>
+        <v>-0.16259236788385</v>
       </c>
       <c r="P23" t="n">
-        <v>26.6520709335994</v>
+        <v>26.6058305315342</v>
       </c>
       <c r="Q23" t="n">
         <v>6.576191</v>
@@ -2039,13 +2039,13 @@
         <v>6.12347377</v>
       </c>
       <c r="U23" t="n">
-        <v>0.0200836386114905</v>
+        <v>0.0196713212942938</v>
       </c>
       <c r="V23" t="n">
-        <v>114.794913561919</v>
+        <v>116.440688212685</v>
       </c>
       <c r="W23" t="n">
-        <v>28.434535649395</v>
+        <v>26.2769064321971</v>
       </c>
     </row>
     <row r="24">
@@ -2053,34 +2053,34 @@
         <v>45</v>
       </c>
       <c r="B24" t="n">
-        <v>143.618503667693</v>
+        <v>158.456214656014</v>
       </c>
       <c r="C24" t="n">
-        <v>29945.3294512391</v>
+        <v>29970.8366330789</v>
       </c>
       <c r="D24" t="n">
-        <v>29801.7109475714</v>
+        <v>29812.3804184229</v>
       </c>
       <c r="E24" t="n">
-        <v>0.481913618719254</v>
+        <v>0.531511447365318</v>
       </c>
       <c r="F24" t="n">
-        <v>131.750565108055</v>
+        <v>126.458795478251</v>
       </c>
       <c r="G24" t="n">
-        <v>-235.745446900706</v>
+        <v>-234.370548739591</v>
       </c>
       <c r="H24" t="n">
-        <v>-110.211724565787</v>
+        <v>-91.4107694578662</v>
       </c>
       <c r="I24" t="n">
-        <v>357.825110026131</v>
+        <v>357.778737375219</v>
       </c>
       <c r="J24" t="n">
-        <v>136.018200467624</v>
+        <v>134.027201173751</v>
       </c>
       <c r="K24" t="n">
-        <v>20.3357964077847</v>
+        <v>21.0194903388027</v>
       </c>
       <c r="L24" t="n">
         <v>0</v>
@@ -2092,10 +2092,10 @@
         <v>0</v>
       </c>
       <c r="O24" t="n">
-        <v>-0.133380385721651</v>
+        <v>-0.17250312765352</v>
       </c>
       <c r="P24" t="n">
-        <v>21.4971801395417</v>
+        <v>21.4493815168303</v>
       </c>
       <c r="Q24" t="n">
         <v>4.63454</v>
@@ -2110,13 +2110,13 @@
         <v>4.0318455</v>
       </c>
       <c r="U24" t="n">
-        <v>-0.0296869521478507</v>
+        <v>-0.0301131638372368</v>
       </c>
       <c r="V24" t="n">
-        <v>124.977556941912</v>
+        <v>129.066996790651</v>
       </c>
       <c r="W24" t="n">
-        <v>29.6511329071376</v>
+        <v>26.9099733466751</v>
       </c>
     </row>
     <row r="25">
@@ -2124,34 +2124,34 @@
         <v>46</v>
       </c>
       <c r="B25" t="n">
-        <v>126.987858841922</v>
+        <v>146.577255612518</v>
       </c>
       <c r="C25" t="n">
-        <v>30256.7723869391</v>
+        <v>30282.5448532737</v>
       </c>
       <c r="D25" t="n">
-        <v>30129.7845280972</v>
+        <v>30135.9675976612</v>
       </c>
       <c r="E25" t="n">
-        <v>0.421469522038898</v>
+        <v>0.486386425581031</v>
       </c>
       <c r="F25" t="n">
-        <v>121.697460124694</v>
+        <v>116.281401340597</v>
       </c>
       <c r="G25" t="n">
-        <v>-231.948610115942</v>
+        <v>-230.649053540686</v>
       </c>
       <c r="H25" t="n">
-        <v>-107.398751306019</v>
+        <v>-85.8398925620384</v>
       </c>
       <c r="I25" t="n">
-        <v>344.637760139189</v>
+        <v>346.784800374646</v>
       </c>
       <c r="J25" t="n">
-        <v>133.478668349959</v>
+        <v>131.485516111743</v>
       </c>
       <c r="K25" t="n">
-        <v>22.7802647724545</v>
+        <v>23.4567988090075</v>
       </c>
       <c r="L25" t="n">
         <v>0</v>
@@ -2163,10 +2163,10 @@
         <v>0</v>
       </c>
       <c r="O25" t="n">
-        <v>-0.261075582377778</v>
+        <v>-0.301493316654216</v>
       </c>
       <c r="P25" t="n">
-        <v>13.6083604702455</v>
+        <v>13.5589796769745</v>
       </c>
       <c r="Q25" t="n">
         <v>2.745007</v>
@@ -2181,13 +2181,13 @@
         <v>2.35332026</v>
       </c>
       <c r="U25" t="n">
-        <v>-0.132815877324287</v>
+        <v>-0.133256196942915</v>
       </c>
       <c r="V25" t="n">
-        <v>132.811414961013</v>
+        <v>139.587694665879</v>
       </c>
       <c r="W25" t="n">
-        <v>28.8221657852194</v>
+        <v>25.5997833646396</v>
       </c>
     </row>
     <row r="26">
@@ -2195,34 +2195,34 @@
         <v>47</v>
       </c>
       <c r="B26" t="n">
-        <v>115.907937747174</v>
+        <v>141.764102555948</v>
       </c>
       <c r="C26" t="n">
-        <v>30562.1364104264</v>
+        <v>30588.168983289</v>
       </c>
       <c r="D26" t="n">
-        <v>30446.2284726792</v>
+        <v>30446.404880733</v>
       </c>
       <c r="E26" t="n">
-        <v>0.380697194896196</v>
+        <v>0.465618529055489</v>
       </c>
       <c r="F26" t="n">
-        <v>123.333196267824</v>
+        <v>117.791396187898</v>
       </c>
       <c r="G26" t="n">
-        <v>-240.579710550137</v>
+        <v>-239.356407054816</v>
       </c>
       <c r="H26" t="n">
-        <v>-100.91780904032</v>
+        <v>-76.5975613113217</v>
       </c>
       <c r="I26" t="n">
-        <v>334.072261069808</v>
+        <v>339.926674734187</v>
       </c>
       <c r="J26" t="n">
-        <v>128.522900966046</v>
+        <v>126.458737196078</v>
       </c>
       <c r="K26" t="n">
-        <v>24.749914378397</v>
+        <v>24.5191547333309</v>
       </c>
       <c r="L26" t="n">
         <v>0</v>
@@ -2234,10 +2234,10 @@
         <v>0</v>
       </c>
       <c r="O26" t="n">
-        <v>-0.526533082628717</v>
+        <v>-0.568270007000294</v>
       </c>
       <c r="P26" t="n">
-        <v>7.28214116683889</v>
+        <v>7.23114863915134</v>
       </c>
       <c r="Q26" t="n">
         <v>0.855474</v>
@@ -2252,13 +2252,13 @@
         <v>2.39286449</v>
       </c>
       <c r="U26" t="n">
-        <v>-0.163310789857231</v>
+        <v>-0.163765481020676</v>
       </c>
       <c r="V26" t="n">
-        <v>136.316621048313</v>
+        <v>146.332384997734</v>
       </c>
       <c r="W26" t="n">
-        <v>27.8220788926986</v>
+        <v>26.0488361659137</v>
       </c>
     </row>
     <row r="27">
@@ -2266,34 +2266,34 @@
         <v>48</v>
       </c>
       <c r="B27" t="n">
-        <v>84.5866982170311</v>
+        <v>113.868718952199</v>
       </c>
       <c r="C27" t="n">
-        <v>30851.8978925676</v>
+        <v>30878.1772818436</v>
       </c>
       <c r="D27" t="n">
-        <v>30767.3111943505</v>
+        <v>30764.3085628914</v>
       </c>
       <c r="E27" t="n">
-        <v>0.274923920659531</v>
+        <v>0.370132547329693</v>
       </c>
       <c r="F27" t="n">
-        <v>111.049070241774</v>
+        <v>105.381227554369</v>
       </c>
       <c r="G27" t="n">
-        <v>-245.620958280058</v>
+        <v>-244.475209556225</v>
       </c>
       <c r="H27" t="n">
-        <v>-101.827745326645</v>
+        <v>-74.7350509611935</v>
       </c>
       <c r="I27" t="n">
-        <v>320.98633158196</v>
+        <v>327.697751915248</v>
       </c>
       <c r="J27" t="n">
-        <v>119.613876795302</v>
+        <v>117.479029704434</v>
       </c>
       <c r="K27" t="n">
-        <v>25.8887120951849</v>
+        <v>25.6506910891258</v>
       </c>
       <c r="L27" t="n">
         <v>0</v>
@@ -2305,10 +2305,10 @@
         <v>0</v>
       </c>
       <c r="O27" t="n">
-        <v>-0.843201232807189</v>
+        <v>-0.886251501522459</v>
       </c>
       <c r="P27" t="n">
-        <v>3.6751382602112</v>
+        <v>3.62254114021558</v>
       </c>
       <c r="Q27" t="n">
         <v>0.573855</v>
@@ -2323,13 +2323,13 @@
         <v>2.42854317</v>
       </c>
       <c r="U27" t="n">
-        <v>-0.190647103038204</v>
+        <v>-0.191116102061576</v>
       </c>
       <c r="V27" t="n">
-        <v>137.856256539387</v>
+        <v>148.529682525638</v>
       </c>
       <c r="W27" t="n">
-        <v>26.6896480577196</v>
+        <v>25.1966268894185</v>
       </c>
     </row>
     <row r="28">
@@ -2337,34 +2337,34 @@
         <v>49</v>
       </c>
       <c r="B28" t="n">
-        <v>77.962632836028</v>
+        <v>111.719970474134</v>
       </c>
       <c r="C28" t="n">
-        <v>31121.5989644067</v>
+        <v>31148.1080828061</v>
       </c>
       <c r="D28" t="n">
-        <v>31043.6363315706</v>
+        <v>31036.3881123319</v>
       </c>
       <c r="E28" t="n">
-        <v>0.251138855008248</v>
+        <v>0.359964471605978</v>
       </c>
       <c r="F28" t="n">
-        <v>103.972456233447</v>
+        <v>98.1991209312138</v>
       </c>
       <c r="G28" t="n">
-        <v>-253.911873797245</v>
+        <v>-252.845245415102</v>
       </c>
       <c r="H28" t="n">
-        <v>-85.0562828329103</v>
+        <v>-55.1277221090837</v>
       </c>
       <c r="I28" t="n">
-        <v>312.958333232736</v>
+        <v>321.493817067106</v>
       </c>
       <c r="J28" t="n">
-        <v>111.209591590338</v>
+        <v>109.004209339996</v>
       </c>
       <c r="K28" t="n">
-        <v>27.0725307916882</v>
+        <v>26.8272560962887</v>
       </c>
       <c r="L28" t="n">
         <v>0</v>
@@ -2376,10 +2376,10 @@
         <v>0</v>
       </c>
       <c r="O28" t="n">
-        <v>-1.14371753839952</v>
+        <v>-1.1880797639057</v>
       </c>
       <c r="P28" t="n">
-        <v>2.45895712130861</v>
+        <v>2.40475710426217</v>
       </c>
       <c r="Q28" t="n">
         <v>0.378236</v>
@@ -2394,13 +2394,13 @@
         <v>2.44287734</v>
       </c>
       <c r="U28" t="n">
-        <v>-0.217981761991116</v>
+        <v>-0.21846505375811</v>
       </c>
       <c r="V28" t="n">
-        <v>141.170161053682</v>
+        <v>153.172502595523</v>
       </c>
       <c r="W28" t="n">
-        <v>25.9219286361102</v>
+        <v>25.0047734086998</v>
       </c>
     </row>
     <row r="29">
@@ -2408,34 +2408,34 @@
         <v>50</v>
       </c>
       <c r="B29" t="n">
-        <v>72.3250134510954</v>
+        <v>108.281409042746</v>
       </c>
       <c r="C29" t="n">
-        <v>31395.1500139805</v>
+        <v>31421.8921408821</v>
       </c>
       <c r="D29" t="n">
-        <v>31322.8250005294</v>
+        <v>31313.6107318394</v>
       </c>
       <c r="E29" t="n">
-        <v>0.23090194913733</v>
+        <v>0.345796624892714</v>
       </c>
       <c r="F29" t="n">
-        <v>95.8870226886498</v>
+        <v>90.0031004433397</v>
       </c>
       <c r="G29" t="n">
-        <v>-260.183715591002</v>
+        <v>-259.198145460597</v>
       </c>
       <c r="H29" t="n">
-        <v>-70.5729936262473</v>
+        <v>-39.4689488172067</v>
       </c>
       <c r="I29" t="n">
-        <v>307.194699979695</v>
+        <v>316.945402877211</v>
       </c>
       <c r="J29" t="n">
-        <v>102.612540224387</v>
+        <v>100.33645140383</v>
       </c>
       <c r="K29" t="n">
-        <v>28.2983243461254</v>
+        <v>28.0457790816801</v>
       </c>
       <c r="L29" t="n">
         <v>0</v>
@@ -2447,10 +2447,10 @@
         <v>0</v>
       </c>
       <c r="O29" t="n">
-        <v>-1.45274975922487</v>
+        <v>-1.4984269945124</v>
       </c>
       <c r="P29" t="n">
-        <v>1.52869440752704</v>
+        <v>1.47288776340651</v>
       </c>
       <c r="Q29" t="n">
         <v>0.211344</v>
@@ -2465,13 +2465,13 @@
         <v>2.45433355</v>
       </c>
       <c r="U29" t="n">
-        <v>-0.245322041437177</v>
+        <v>-0.245819659207739</v>
       </c>
       <c r="V29" t="n">
-        <v>145.952613868636</v>
+        <v>158.869116097009</v>
       </c>
       <c r="W29" t="n">
-        <v>25.3736963836805</v>
+        <v>24.8385126350053</v>
       </c>
     </row>
     <row r="30">
@@ -2479,34 +2479,34 @@
         <v>51</v>
       </c>
       <c r="B30" t="n">
-        <v>55.049891021277</v>
+        <v>95.9269937569424</v>
       </c>
       <c r="C30" t="n">
-        <v>31679.947051148</v>
+        <v>31706.9317657902</v>
       </c>
       <c r="D30" t="n">
-        <v>31624.8971601267</v>
+        <v>31611.0047720333</v>
       </c>
       <c r="E30" t="n">
-        <v>0.174071367702933</v>
+        <v>0.303460755039997</v>
       </c>
       <c r="F30" t="n">
-        <v>89.6636110116705</v>
+        <v>83.6637571091378</v>
       </c>
       <c r="G30" t="n">
-        <v>-270.544626821313</v>
+        <v>-269.64297540776</v>
       </c>
       <c r="H30" t="n">
-        <v>-62.5888323620248</v>
+        <v>-31.0708179911747</v>
       </c>
       <c r="I30" t="n">
-        <v>298.519739192945</v>
+        <v>312.977030046739</v>
       </c>
       <c r="J30" t="n">
-        <v>94.2028539692205</v>
+        <v>91.8558272158848</v>
       </c>
       <c r="K30" t="n">
-        <v>29.5658944065828</v>
+        <v>29.3060557896192</v>
       </c>
       <c r="L30" t="n">
         <v>0</v>
@@ -2518,10 +2518,10 @@
         <v>0</v>
       </c>
       <c r="O30" t="n">
-        <v>-1.79445229368442</v>
+        <v>-1.84144865954343</v>
       </c>
       <c r="P30" t="n">
-        <v>-3.8920620190091</v>
+        <v>0.604569175177438</v>
       </c>
       <c r="Q30" t="n">
         <v>-0.00499800000000003</v>
@@ -2536,13 +2536,13 @@
         <v>1.91853524</v>
       </c>
       <c r="U30" t="n">
-        <v>-0.27266962342627</v>
+        <v>-0.273181612093186</v>
       </c>
       <c r="V30" t="n">
-        <v>152.227588993455</v>
+        <v>165.331459763613</v>
       </c>
       <c r="W30" t="n">
-        <v>25.0461635198057</v>
+        <v>24.557326134081</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update to Levels Code
</commit_message>
<xml_diff>
--- a/fim_levels.xlsx
+++ b/fim_levels.xlsx
@@ -12,30 +12,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t xml:space="preserve">date</t>
   </si>
   <si>
-    <t xml:space="preserve">minus_neutral_sum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">real_gdp_actual</t>
-  </si>
-  <si>
-    <t xml:space="preserve">federal_purchases_contribution_levels</t>
-  </si>
-  <si>
-    <t xml:space="preserve">state_purchases_contribution_levels</t>
-  </si>
-  <si>
-    <t xml:space="preserve">federal_levels</t>
-  </si>
-  <si>
-    <t xml:space="preserve">state_levels</t>
-  </si>
-  <si>
-    <t xml:space="preserve">consumption_levels</t>
+    <t xml:space="preserve">real_federal_levels</t>
+  </si>
+  <si>
+    <t xml:space="preserve">real_state_levels</t>
+  </si>
+  <si>
+    <t xml:space="preserve">real_consumption_levels</t>
+  </si>
+  <si>
+    <t xml:space="preserve">real_delta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">real_gdp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">real_gdp_counterfactual</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2019 Q4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020 Q1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020 Q2</t>
   </si>
   <si>
     <t xml:space="preserve">2020 Q3</t>
@@ -90,6 +96,24 @@
   </si>
   <si>
     <t xml:space="preserve">2024 Q4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025 Q1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025 Q2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025 Q3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025 Q4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2026 Q1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2026 Q2</t>
   </si>
 </sst>
 </file>
@@ -443,452 +467,616 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2"/>
-      <c r="C2" t="n">
-        <v>20548.8</v>
-      </c>
+      <c r="C2"/>
       <c r="D2"/>
       <c r="E2"/>
-      <c r="F2"/>
+      <c r="F2" t="n">
+        <v>20985.4</v>
+      </c>
       <c r="G2"/>
-      <c r="H2"/>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3"/>
+        <v>8</v>
+      </c>
+      <c r="B3" t="n">
+        <v>9.11611259734197</v>
+      </c>
       <c r="C3" t="n">
-        <v>20771.7</v>
-      </c>
-      <c r="D3"/>
-      <c r="E3"/>
-      <c r="F3"/>
-      <c r="G3"/>
-      <c r="H3"/>
+        <v>12.5638612399199</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1.97165989424524</v>
+      </c>
+      <c r="E3" t="n">
+        <v>23.6516337315071</v>
+      </c>
+      <c r="F3" t="n">
+        <v>20693.2</v>
+      </c>
+      <c r="G3" t="n">
+        <v>20669.5483662685</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" t="n">
-        <v>431.185666162402</v>
+        <v>207.649728878123</v>
       </c>
       <c r="C4" t="n">
-        <v>21058.4</v>
+        <v>-119.587933896327</v>
       </c>
       <c r="D4" t="n">
-        <v>55.4704736178442</v>
+        <v>673.745301791097</v>
       </c>
       <c r="E4" t="n">
-        <v>-22.5937312132396</v>
+        <v>761.807096772892</v>
       </c>
       <c r="F4" t="n">
-        <v>68.2860748251505</v>
+        <v>19056.6</v>
       </c>
       <c r="G4" t="n">
-        <v>-35.409332420546</v>
-      </c>
-      <c r="H4" t="n">
-        <v>398.308923757797</v>
+        <v>18294.7929032271</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" t="n">
-        <v>311.619199745308</v>
+        <v>127.979290104342</v>
       </c>
       <c r="C5" t="n">
-        <v>21389</v>
+        <v>-116.533471533985</v>
       </c>
       <c r="D5" t="n">
-        <v>14.9763320644106</v>
+        <v>884.390394228708</v>
       </c>
       <c r="E5" t="n">
-        <v>-47.2596022174325</v>
+        <v>895.836212799064</v>
       </c>
       <c r="F5" t="n">
-        <v>56.2424604441046</v>
+        <v>20548.8</v>
       </c>
       <c r="G5" t="n">
-        <v>-88.5257305971265</v>
-      </c>
-      <c r="H5" t="n">
-        <v>343.90246989833</v>
+        <v>19652.9637872009</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" t="n">
-        <v>151.392287085526</v>
+        <v>111.031299475772</v>
       </c>
       <c r="C6" t="n">
-        <v>21571.4</v>
+        <v>-131.371282522965</v>
       </c>
       <c r="D6" t="n">
-        <v>-24.2582885782388</v>
+        <v>745.367542422039</v>
       </c>
       <c r="E6" t="n">
-        <v>-46.4558674110699</v>
+        <v>725.027559374846</v>
       </c>
       <c r="F6" t="n">
-        <v>22.8729508070367</v>
+        <v>20771.7</v>
       </c>
       <c r="G6" t="n">
-        <v>-93.5871067963453</v>
-      </c>
-      <c r="H6" t="n">
-        <v>222.106443074835</v>
+        <v>20046.6724406252</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7" t="n">
-        <v>-13.9087649675352</v>
+        <v>176.416517092735</v>
       </c>
       <c r="C7" t="n">
-        <v>21960.4</v>
+        <v>-163.481976228782</v>
       </c>
       <c r="D7" t="n">
-        <v>-20.7399636946732</v>
+        <v>1123.03655616054</v>
       </c>
       <c r="E7" t="n">
-        <v>-77.0060489939665</v>
+        <v>1135.9710970245</v>
       </c>
       <c r="F7" t="n">
-        <v>44.9956974060643</v>
+        <v>21058.4</v>
       </c>
       <c r="G7" t="n">
-        <v>-142.741710094704</v>
-      </c>
-      <c r="H7" t="n">
-        <v>83.8372477211044</v>
+        <v>19922.4289029755</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" t="n">
-        <v>-247.437525731412</v>
+        <v>165.706488573653</v>
       </c>
       <c r="C8" t="n">
-        <v>21903.9</v>
+        <v>-209.642083210371</v>
       </c>
       <c r="D8" t="n">
-        <v>-66.1756826568537</v>
+        <v>1070.67157246815</v>
       </c>
       <c r="E8" t="n">
-        <v>-94.4679874994422</v>
+        <v>1026.73597783143</v>
       </c>
       <c r="F8" t="n">
-        <v>21.5276501713095</v>
+        <v>21389</v>
       </c>
       <c r="G8" t="n">
-        <v>-182.171320327605</v>
-      </c>
-      <c r="H8" t="n">
-        <v>-86.7938555751159</v>
+        <v>20362.2640221686</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B9" t="n">
-        <v>-542.1513500334</v>
+        <v>135.4353200492</v>
       </c>
       <c r="C9" t="n">
-        <v>21919.2</v>
+        <v>-213.358132555454</v>
       </c>
       <c r="D9" t="n">
-        <v>-90.1819065468524</v>
+        <v>959.067576170796</v>
       </c>
       <c r="E9" t="n">
-        <v>-116.236103528782</v>
+        <v>881.144763664541</v>
       </c>
       <c r="F9" t="n">
-        <v>50.7827488748549</v>
+        <v>21571.4</v>
       </c>
       <c r="G9" t="n">
-        <v>-257.200758950489</v>
-      </c>
-      <c r="H9" t="n">
-        <v>-335.733339957765</v>
+        <v>20690.2552363355</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B10" t="n">
-        <v>-698.708232921434</v>
+        <v>156.123482215256</v>
       </c>
       <c r="C10" t="n">
-        <v>22066.8</v>
+        <v>-253.610710866958</v>
       </c>
       <c r="D10" t="n">
-        <v>-102.740875156754</v>
+        <v>835.591187277986</v>
       </c>
       <c r="E10" t="n">
-        <v>-113.472966771887</v>
+        <v>738.103958626284</v>
       </c>
       <c r="F10" t="n">
-        <v>17.5433872574299</v>
+        <v>21960.4</v>
       </c>
       <c r="G10" t="n">
-        <v>-233.75722918607</v>
-      </c>
-      <c r="H10" t="n">
-        <v>-482.494390992793</v>
+        <v>21222.2960413737</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B11" t="n">
-        <v>-723.090401635941</v>
+        <v>135.684841982149</v>
       </c>
       <c r="C11" t="n">
-        <v>22249.5</v>
+        <v>-283.864546289976</v>
       </c>
       <c r="D11" t="n">
-        <v>-77.5601780094385</v>
+        <v>687.876530584834</v>
       </c>
       <c r="E11" t="n">
-        <v>-106.506747647906</v>
+        <v>539.696826277007</v>
       </c>
       <c r="F11" t="n">
-        <v>6.60701757222026</v>
+        <v>21903.9</v>
       </c>
       <c r="G11" t="n">
-        <v>-190.673943229564</v>
-      </c>
-      <c r="H11" t="n">
-        <v>-539.023475978597</v>
+        <v>21364.203173723</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B12" t="n">
-        <v>-732.580965867739</v>
+        <v>162.607983568493</v>
       </c>
       <c r="C12" t="n">
-        <v>22403.4</v>
+        <v>-339.197695728974</v>
       </c>
       <c r="D12" t="n">
-        <v>-68.755094673</v>
+        <v>478.065051031219</v>
       </c>
       <c r="E12" t="n">
-        <v>-85.0713250369708</v>
+        <v>301.475338870738</v>
       </c>
       <c r="F12" t="n">
-        <v>5.80835095298728</v>
+        <v>21919.2</v>
       </c>
       <c r="G12" t="n">
-        <v>-159.634770662958</v>
-      </c>
-      <c r="H12" t="n">
-        <v>-578.754546157768</v>
+        <v>21617.7246611293</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B13" t="n">
-        <v>-780.530367084103</v>
+        <v>132.941044652791</v>
       </c>
       <c r="C13" t="n">
-        <v>22539.4</v>
+        <v>-320.802371480769</v>
       </c>
       <c r="D13" t="n">
-        <v>-84.2386290276195</v>
+        <v>360.15378479819</v>
       </c>
       <c r="E13" t="n">
-        <v>-62.9663550579417</v>
+        <v>172.292457970213</v>
       </c>
       <c r="F13" t="n">
-        <v>-15.4658566747318</v>
+        <v>22066.8</v>
       </c>
       <c r="G13" t="n">
-        <v>-131.739127410829</v>
-      </c>
-      <c r="H13" t="n">
-        <v>-633.325382998542</v>
+        <v>21894.5075420298</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B14" t="n">
-        <v>-783.699070045889</v>
+        <v>123.436518926475</v>
       </c>
       <c r="C14" t="n">
-        <v>22780.9</v>
+        <v>-286.882030441939</v>
       </c>
       <c r="D14" t="n">
-        <v>-72.6460015441874</v>
+        <v>320.648050057576</v>
       </c>
       <c r="E14" t="n">
-        <v>-37.8900529647731</v>
+        <v>157.202538542112</v>
       </c>
       <c r="F14" t="n">
-        <v>-26.6786689006642</v>
+        <v>22249.5</v>
       </c>
       <c r="G14" t="n">
-        <v>-83.8573856082962</v>
-      </c>
-      <c r="H14" t="n">
-        <v>-673.163015536928</v>
+        <v>22092.2974614579</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B15" t="n">
-        <v>-822.802521669327</v>
+        <v>121.958366138466</v>
       </c>
       <c r="C15" t="n">
-        <v>22960.6</v>
+        <v>-263.55612413089</v>
       </c>
       <c r="D15" t="n">
-        <v>-85.4488151746471</v>
+        <v>296.036157458968</v>
       </c>
       <c r="E15" t="n">
-        <v>-10.7939578547789</v>
+        <v>154.438399466544</v>
       </c>
       <c r="F15" t="n">
-        <v>-25.6880694889519</v>
+        <v>22403.4</v>
       </c>
       <c r="G15" t="n">
-        <v>-70.5547035404741</v>
-      </c>
-      <c r="H15" t="n">
-        <v>-726.559748639901</v>
+        <v>22248.9616005335</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B16" t="n">
-        <v>-835.150346928779</v>
+        <v>103.359459414189</v>
       </c>
       <c r="C16" t="n">
-        <v>23053.5</v>
+        <v>-243.031795235908</v>
       </c>
       <c r="D16" t="n">
-        <v>-98.6555696855141</v>
+        <v>258.471472105083</v>
       </c>
       <c r="E16" t="n">
-        <v>-5.34742908492808</v>
+        <v>118.799136283364</v>
       </c>
       <c r="F16" t="n">
-        <v>-43.3070721856449</v>
+        <v>22539.4</v>
       </c>
       <c r="G16" t="n">
-        <v>-60.6959265847973</v>
-      </c>
-      <c r="H16" t="n">
-        <v>-731.147348158337</v>
+        <v>22420.6008637166</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B17" t="n">
-        <v>-836.898959344985</v>
+        <v>95.0066785256174</v>
       </c>
       <c r="C17" t="n">
-        <v>23223.9</v>
+        <v>-204.887840595535</v>
       </c>
       <c r="D17" t="n">
-        <v>-91.1501573234277</v>
+        <v>233.454459103372</v>
       </c>
       <c r="E17" t="n">
-        <v>-5.44687922348021</v>
+        <v>123.573297033455</v>
       </c>
       <c r="F17" t="n">
-        <v>-34.3705063343748</v>
+        <v>22780.9</v>
       </c>
       <c r="G17" t="n">
-        <v>-62.2265302125331</v>
-      </c>
-      <c r="H17" t="n">
-        <v>-740.301922798077</v>
+        <v>22657.3267029665</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B18" t="n">
-        <v>-811.13852204962</v>
+        <v>95.9468002385108</v>
       </c>
       <c r="C18" t="n">
-        <v>23400.3</v>
+        <v>-195.083665604709</v>
       </c>
       <c r="D18" t="n">
-        <v>-62.7938171881224</v>
+        <v>196.276495906559</v>
       </c>
       <c r="E18" t="n">
-        <v>-0.997234269220371</v>
+        <v>97.1396305403602</v>
       </c>
       <c r="F18" t="n">
-        <v>9.90521544738881</v>
+        <v>22960.6</v>
       </c>
       <c r="G18" t="n">
-        <v>-73.6962669047316</v>
-      </c>
-      <c r="H18" t="n">
-        <v>-747.347470592277</v>
+        <v>22863.4603694596</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" t="n">
+        <v>82.5807197034934</v>
+      </c>
+      <c r="C19" t="n">
+        <v>-187.656271021669</v>
+      </c>
+      <c r="D19" t="n">
+        <v>202.07534968858</v>
+      </c>
+      <c r="E19" t="n">
+        <v>96.999798370405</v>
+      </c>
+      <c r="F19" t="n">
+        <v>23053.5</v>
+      </c>
+      <c r="G19" t="n">
+        <v>22956.5002016296</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
         <v>25</v>
       </c>
-      <c r="B19" t="n">
-        <v>-797.837285833443</v>
-      </c>
-      <c r="C19" t="n">
+      <c r="B20" t="n">
+        <v>90.5671094243449</v>
+      </c>
+      <c r="C20" t="n">
+        <v>-189.520509582592</v>
+      </c>
+      <c r="D20" t="n">
+        <v>202.972948368087</v>
+      </c>
+      <c r="E20" t="n">
+        <v>104.01954820984</v>
+      </c>
+      <c r="F20" t="n">
+        <v>23223.9</v>
+      </c>
+      <c r="G20" t="n">
+        <v>23119.8804517902</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" t="n">
+        <v>126.91537743635</v>
+      </c>
+      <c r="C21" t="n">
+        <v>-198.934760293195</v>
+      </c>
+      <c r="D21" t="n">
+        <v>204.172479097425</v>
+      </c>
+      <c r="E21" t="n">
+        <v>132.153096240581</v>
+      </c>
+      <c r="F21" t="n">
+        <v>23400.3</v>
+      </c>
+      <c r="G21" t="n">
+        <v>23268.1469037594</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" t="n">
+        <v>128.759777630976</v>
+      </c>
+      <c r="C22" t="n">
+        <v>-199.447839359107</v>
+      </c>
+      <c r="D22" t="n">
+        <v>221.518315551549</v>
+      </c>
+      <c r="E22" t="n">
+        <v>150.830253823418</v>
+      </c>
+      <c r="F22" t="n">
         <v>23530.9</v>
       </c>
-      <c r="D19" t="n">
-        <v>-59.154063865707</v>
-      </c>
-      <c r="E19" t="n">
-        <v>-2.97224787235837</v>
-      </c>
-      <c r="F19" t="n">
-        <v>11.5604184314929</v>
-      </c>
-      <c r="G19" t="n">
-        <v>-73.6867301695583</v>
-      </c>
-      <c r="H19" t="n">
-        <v>-735.710974095377</v>
+      <c r="G22" t="n">
+        <v>23380.0697461766</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23" t="n">
+        <v>90.4865795156256</v>
+      </c>
+      <c r="C23" t="n">
+        <v>-191.119873878575</v>
+      </c>
+      <c r="D23" t="n">
+        <v>221.242188082269</v>
+      </c>
+      <c r="E23" t="n">
+        <v>120.60889371932</v>
+      </c>
+      <c r="F23" t="n">
+        <v>23646.7536121738</v>
+      </c>
+      <c r="G23" t="n">
+        <v>23526.1447184545</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24" t="n">
+        <v>64.7837013182723</v>
+      </c>
+      <c r="C24" t="n">
+        <v>-191.934358432925</v>
+      </c>
+      <c r="D24" t="n">
+        <v>225.894484670454</v>
+      </c>
+      <c r="E24" t="n">
+        <v>98.7438275558006</v>
+      </c>
+      <c r="F24" t="n">
+        <v>23765.7113401448</v>
+      </c>
+      <c r="G24" t="n">
+        <v>23666.967512589</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25" t="n">
+        <v>52.554932377094</v>
+      </c>
+      <c r="C25" t="n">
+        <v>-200.553430650199</v>
+      </c>
+      <c r="D25" t="n">
+        <v>238.683673053146</v>
+      </c>
+      <c r="E25" t="n">
+        <v>90.6851747800411</v>
+      </c>
+      <c r="F25" t="n">
+        <v>23876.9588450065</v>
+      </c>
+      <c r="G25" t="n">
+        <v>23786.2736702265</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" t="n">
+        <v>37.1903635853186</v>
+      </c>
+      <c r="C26" t="n">
+        <v>-206.195324818472</v>
+      </c>
+      <c r="D26" t="n">
+        <v>242.06827669853</v>
+      </c>
+      <c r="E26" t="n">
+        <v>73.0633154653769</v>
+      </c>
+      <c r="F26" t="n">
+        <v>23979.8953301531</v>
+      </c>
+      <c r="G26" t="n">
+        <v>23906.8320146878</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>32</v>
+      </c>
+      <c r="B27" t="n">
+        <v>25.7520315518833</v>
+      </c>
+      <c r="C27" t="n">
+        <v>-214.814359231428</v>
+      </c>
+      <c r="D27" t="n">
+        <v>255.0767125584</v>
+      </c>
+      <c r="E27" t="n">
+        <v>66.0143848788558</v>
+      </c>
+      <c r="F27" t="n">
+        <v>24089.0400468942</v>
+      </c>
+      <c r="G27" t="n">
+        <v>24023.0256620154</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>33</v>
+      </c>
+      <c r="B28" t="n">
+        <v>12.0582807583151</v>
+      </c>
+      <c r="C28" t="n">
+        <v>-222.254393456349</v>
+      </c>
+      <c r="D28" t="n">
+        <v>264.682250155971</v>
+      </c>
+      <c r="E28" t="n">
+        <v>54.4861374579374</v>
+      </c>
+      <c r="F28" t="n">
+        <v>24201.2888794325</v>
+      </c>
+      <c r="G28" t="n">
+        <v>24146.8027419746</v>
       </c>
     </row>
   </sheetData>

</xml_diff>